<commit_message>
Create "Ones Players to Watch" and bracket simulation [ON PROGRESS]
</commit_message>
<xml_diff>
--- a/worldcup-master/data-csv/fixtures_stadium.xlsx
+++ b/worldcup-master/data-csv/fixtures_stadium.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\World-Cup-2026-\worldcup-master\data-csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620D8CC9-EBED-411D-A210-6B140605FD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FFCB02-D995-44AC-8321-5FED98BF2FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="600" windowWidth="14115" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1107,18 +1107,9 @@
     <t>away_team_id</t>
   </si>
   <si>
-    <t>Group A Runners-up</t>
-  </si>
-  <si>
-    <t>Group B Runners-up</t>
-  </si>
-  <si>
     <t>Round of 32</t>
   </si>
   <si>
-    <t>Group E Winners</t>
-  </si>
-  <si>
     <t>Group A/B/C/D/F 3rd Place</t>
   </si>
   <si>
@@ -1137,177 +1128,27 @@
     <t>Final</t>
   </si>
   <si>
-    <t>Group F Winners</t>
-  </si>
-  <si>
-    <t>Group C Runners-up</t>
-  </si>
-  <si>
-    <t>Group C Winners</t>
-  </si>
-  <si>
-    <t>Group F Runners-up</t>
-  </si>
-  <si>
-    <t>Group I Winners</t>
-  </si>
-  <si>
     <t>Group C/D/F/G/H 3rd Place</t>
   </si>
   <si>
-    <t>Group E Runners-up</t>
-  </si>
-  <si>
-    <t>Group I Runners-up</t>
-  </si>
-  <si>
-    <t>Group A Winners</t>
-  </si>
-  <si>
     <t>Group C/E/F/H/I 3rd Place</t>
   </si>
   <si>
-    <t>Group L Winners</t>
-  </si>
-  <si>
     <t>Group E/H/I/J/K 3rd Place</t>
   </si>
   <si>
-    <t>Group D Winners</t>
-  </si>
-  <si>
     <t>Group B/E/F/I/J 3rd Place</t>
   </si>
   <si>
-    <t>Group G Winners</t>
-  </si>
-  <si>
     <t>Group A/E/H/I/J 3rd Place</t>
   </si>
   <si>
-    <t>Group K Runners-up</t>
-  </si>
-  <si>
-    <t>Group L Runners-up</t>
-  </si>
-  <si>
-    <t>Group H Winners</t>
-  </si>
-  <si>
-    <t>Group J Runners-up</t>
-  </si>
-  <si>
-    <t>Group B Winners</t>
-  </si>
-  <si>
-    <t>Group K Winners</t>
-  </si>
-  <si>
     <t>Group E/F/G/I/J 3rd Place</t>
   </si>
   <si>
-    <t>Group J Winners</t>
-  </si>
-  <si>
-    <t>Group H Runners-up</t>
-  </si>
-  <si>
     <t>Group D/E/I/J/L 3rd Place</t>
   </si>
   <si>
-    <t>Group D Runners-up</t>
-  </si>
-  <si>
-    <t>Group G Runners-up</t>
-  </si>
-  <si>
-    <t>Winner Match 74</t>
-  </si>
-  <si>
-    <t>Winner Match 77</t>
-  </si>
-  <si>
-    <t>Winner Match 73</t>
-  </si>
-  <si>
-    <t>Winner Match 75</t>
-  </si>
-  <si>
-    <t>Winner Match 78</t>
-  </si>
-  <si>
-    <t>Winner Match 76</t>
-  </si>
-  <si>
-    <t>Winner Match 79</t>
-  </si>
-  <si>
-    <t>Winner Match 80</t>
-  </si>
-  <si>
-    <t>Winner Match 84</t>
-  </si>
-  <si>
-    <t>Winner Match 83</t>
-  </si>
-  <si>
-    <t>Winner Match 81</t>
-  </si>
-  <si>
-    <t>Winner Match 82</t>
-  </si>
-  <si>
-    <t>Winner Match 86</t>
-  </si>
-  <si>
-    <t>Winner Match 85</t>
-  </si>
-  <si>
-    <t>Winner Match 89</t>
-  </si>
-  <si>
-    <t>Winner Match 93</t>
-  </si>
-  <si>
-    <t>Winner Match 91</t>
-  </si>
-  <si>
-    <t>Winner Match 95</t>
-  </si>
-  <si>
-    <t>Winner Match 99</t>
-  </si>
-  <si>
-    <t>Winner Match 97</t>
-  </si>
-  <si>
-    <t>Winner Match 101</t>
-  </si>
-  <si>
-    <t>Winner Match 88</t>
-  </si>
-  <si>
-    <t>Winner Match 87</t>
-  </si>
-  <si>
-    <t>Winner Match 90</t>
-  </si>
-  <si>
-    <t>Winner Match 94</t>
-  </si>
-  <si>
-    <t>Winner Match 92</t>
-  </si>
-  <si>
-    <t>Winner Match 96</t>
-  </si>
-  <si>
-    <t>Winner Match 98</t>
-  </si>
-  <si>
-    <t>Winner Match 100</t>
-  </si>
-  <si>
     <t>stadium</t>
   </si>
   <si>
@@ -1326,19 +1167,178 @@
     <t>San Fransisco</t>
   </si>
   <si>
-    <t>Runner-up Match 101</t>
-  </si>
-  <si>
-    <t>Runner-up Match 102</t>
-  </si>
-  <si>
-    <t>Winner Match 102</t>
-  </si>
-  <si>
     <t>Miami</t>
   </si>
   <si>
     <t>T-99</t>
+  </si>
+  <si>
+    <t>Group B 2nd Place</t>
+  </si>
+  <si>
+    <t>Group C 2nd Place</t>
+  </si>
+  <si>
+    <t>Group F 2nd Place</t>
+  </si>
+  <si>
+    <t>Group I 2nd Place</t>
+  </si>
+  <si>
+    <t>Group L 2nd Place</t>
+  </si>
+  <si>
+    <t>Group J 2nd Place</t>
+  </si>
+  <si>
+    <t>Group H 2nd Place</t>
+  </si>
+  <si>
+    <t>Group G 2nd Place</t>
+  </si>
+  <si>
+    <t>Group A 2nd Place</t>
+  </si>
+  <si>
+    <t>Group E 2nd Place</t>
+  </si>
+  <si>
+    <t>Group K 2nd Place</t>
+  </si>
+  <si>
+    <t>Group D 2nd Place</t>
+  </si>
+  <si>
+    <t>Group E 1st Place</t>
+  </si>
+  <si>
+    <t>Group F 1st Place</t>
+  </si>
+  <si>
+    <t>Group C 1st Place</t>
+  </si>
+  <si>
+    <t>Group I 1st Place</t>
+  </si>
+  <si>
+    <t>Group A 1st Place</t>
+  </si>
+  <si>
+    <t>Group L 1st Place</t>
+  </si>
+  <si>
+    <t>Group D 1st Place</t>
+  </si>
+  <si>
+    <t>Group G 1st Place</t>
+  </si>
+  <si>
+    <t>Group H 1st Place</t>
+  </si>
+  <si>
+    <t>Group B 1st Place</t>
+  </si>
+  <si>
+    <t>Group J 1st Place</t>
+  </si>
+  <si>
+    <t>Group K 1st Place</t>
+  </si>
+  <si>
+    <t>Winner M-74</t>
+  </si>
+  <si>
+    <t>Winner M-73</t>
+  </si>
+  <si>
+    <t>Winner M-76</t>
+  </si>
+  <si>
+    <t>Winner M-79</t>
+  </si>
+  <si>
+    <t>Winner M-83</t>
+  </si>
+  <si>
+    <t>Winner M-81</t>
+  </si>
+  <si>
+    <t>Winner M-86</t>
+  </si>
+  <si>
+    <t>Winner M-85</t>
+  </si>
+  <si>
+    <t>Winner M-89</t>
+  </si>
+  <si>
+    <t>Winner M-93</t>
+  </si>
+  <si>
+    <t>Winner M-91</t>
+  </si>
+  <si>
+    <t>Winner M-95</t>
+  </si>
+  <si>
+    <t>Winner M-97</t>
+  </si>
+  <si>
+    <t>Winner M-99</t>
+  </si>
+  <si>
+    <t>Runner-up M-101</t>
+  </si>
+  <si>
+    <t>Winner M-101</t>
+  </si>
+  <si>
+    <t>Winner M-77</t>
+  </si>
+  <si>
+    <t>Winner M-75</t>
+  </si>
+  <si>
+    <t>Winner M-78</t>
+  </si>
+  <si>
+    <t>Winner M-80</t>
+  </si>
+  <si>
+    <t>Winner M-84</t>
+  </si>
+  <si>
+    <t>Winner M-82</t>
+  </si>
+  <si>
+    <t>Winner M-88</t>
+  </si>
+  <si>
+    <t>Winner M-87</t>
+  </si>
+  <si>
+    <t>Winner M-90</t>
+  </si>
+  <si>
+    <t>Winner M-94</t>
+  </si>
+  <si>
+    <t>Winner M-92</t>
+  </si>
+  <si>
+    <t>Winner M-96</t>
+  </si>
+  <si>
+    <t>Winner M-98</t>
+  </si>
+  <si>
+    <t>Winner M-100</t>
+  </si>
+  <si>
+    <t>Runner-up M-102</t>
+  </si>
+  <si>
+    <t>Winner M-102</t>
   </si>
 </sst>
 </file>
@@ -1383,9 +1383,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1428,6 +1425,9 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1443,7 +1443,18 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1433277F-7F70-46C8-9FA7-2F397B0BD689}" name="fixtures" displayName="fixtures" ref="A1:K105" totalsRowShown="0">
-  <autoFilter ref="A1:K105" xr:uid="{1433277F-7F70-46C8-9FA7-2F397B0BD689}"/>
+  <autoFilter ref="A1:K105" xr:uid="{1433277F-7F70-46C8-9FA7-2F397B0BD689}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Bronze Final"/>
+        <filter val="Final"/>
+        <filter val="Quarter-Finals"/>
+        <filter val="Round of 16"/>
+        <filter val="Round of 32"/>
+        <filter val="Semi-Finals"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{56F78C62-1BC2-4561-B5A5-EA107AE1F787}" name="key_id"/>
     <tableColumn id="2" xr3:uid="{0DA00091-7DE3-4153-A570-4B8F11B972C6}" name="home_team"/>
@@ -1456,8 +1467,8 @@
     </tableColumn>
     <tableColumn id="6" xr3:uid="{204A6E4B-0B10-468F-A07B-F3642A529AF0}" name="city"/>
     <tableColumn id="11" xr3:uid="{29641C71-D295-4E01-A048-2BA01B6B87EB}" name="stadium"/>
-    <tableColumn id="7" xr3:uid="{B18026C7-BD02-47DA-B6CE-A87B0F6F2433}" name="stadium_id" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{09DF7FE1-13D9-4515-B7DB-C04EBDF681AD}" name="date" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B18026C7-BD02-47DA-B6CE-A87B0F6F2433}" name="stadium_id" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{09DF7FE1-13D9-4515-B7DB-C04EBDF681AD}" name="date" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{77F21709-473D-48DB-9E5F-C94D6710E980}" name="group"/>
     <tableColumn id="10" xr3:uid="{11BCE8D4-C613-447C-9304-B595B8D05786}" name="phase"/>
   </tableColumns>
@@ -1730,19 +1741,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1765,10 +1776,10 @@
         <v>354</v>
       </c>
       <c r="F1" t="s">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="G1" t="s">
-        <v>422</v>
+        <v>369</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1795,7 +1806,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1844,7 +1855,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1893,7 +1904,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1942,7 +1953,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1991,7 +2002,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2013,7 +2024,7 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H6" t="s">
         <v>64</v>
@@ -2040,7 +2051,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2089,7 +2100,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2108,7 +2119,7 @@
         <v>T-47</v>
       </c>
       <c r="F8" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
@@ -2138,7 +2149,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2157,10 +2168,10 @@
         <v>T-75</v>
       </c>
       <c r="F9" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G9" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H9" t="s">
         <v>62</v>
@@ -2187,7 +2198,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2236,7 +2247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2285,7 +2296,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2334,7 +2345,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2383,7 +2394,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2402,7 +2413,7 @@
         <v>T-84</v>
       </c>
       <c r="F14" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G14" t="s">
         <v>69</v>
@@ -2432,7 +2443,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2481,7 +2492,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2530,7 +2541,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2579,7 +2590,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2598,7 +2609,7 @@
         <v>T-65</v>
       </c>
       <c r="F18" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G18" t="s">
         <v>54</v>
@@ -2628,7 +2639,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2650,7 +2661,7 @@
         <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H19" t="s">
         <v>64</v>
@@ -2677,7 +2688,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2726,7 +2737,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2745,10 +2756,10 @@
         <v>T-91</v>
       </c>
       <c r="F21" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G21" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H21" t="s">
         <v>62</v>
@@ -2775,7 +2786,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2824,7 +2835,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2873,7 +2884,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2922,7 +2933,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2971,7 +2982,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3020,7 +3031,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3069,7 +3080,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3118,7 +3129,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3167,7 +3178,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3216,7 +3227,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3238,7 +3249,7 @@
         <v>34</v>
       </c>
       <c r="G31" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H31" t="s">
         <v>64</v>
@@ -3265,7 +3276,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3284,10 +3295,10 @@
         <v>T-55</v>
       </c>
       <c r="F32" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G32" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H32" t="s">
         <v>62</v>
@@ -3314,7 +3325,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3363,7 +3374,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3412,7 +3423,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3461,7 +3472,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3510,7 +3521,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3559,7 +3570,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3578,7 +3589,7 @@
         <v>T-90</v>
       </c>
       <c r="F38" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G38" t="s">
         <v>69</v>
@@ -3608,7 +3619,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3657,7 +3668,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3706,7 +3717,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3755,7 +3766,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3774,7 +3785,7 @@
         <v>T-65</v>
       </c>
       <c r="F42" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G42" t="s">
         <v>54</v>
@@ -3804,7 +3815,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3902,7 +3913,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3921,10 +3932,10 @@
         <v>T-01</v>
       </c>
       <c r="F45" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G45" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H45" t="s">
         <v>62</v>
@@ -3951,7 +3962,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3973,7 +3984,7 @@
         <v>34</v>
       </c>
       <c r="G46" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H46" t="s">
         <v>64</v>
@@ -4000,7 +4011,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4049,7 +4060,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4098,7 +4109,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4147,7 +4158,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4166,7 +4177,7 @@
         <v>T-09</v>
       </c>
       <c r="F50" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G50" t="s">
         <v>69</v>
@@ -4196,7 +4207,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4245,7 +4256,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4294,7 +4305,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4343,7 +4354,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4392,7 +4403,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4441,7 +4452,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4490,7 +4501,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4509,7 +4520,7 @@
         <v>T-31</v>
       </c>
       <c r="F57" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G57" t="s">
         <v>54</v>
@@ -4539,7 +4550,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4588,7 +4599,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4637,7 +4648,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4686,7 +4697,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4705,10 +4716,10 @@
         <v>T-04</v>
       </c>
       <c r="F61" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G61" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H61" t="s">
         <v>62</v>
@@ -4735,7 +4746,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4757,7 +4768,7 @@
         <v>34</v>
       </c>
       <c r="G62" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H62" t="s">
         <v>64</v>
@@ -4784,7 +4795,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4833,7 +4844,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4882,7 +4893,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4931,7 +4942,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4980,7 +4991,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5029,7 +5040,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5048,7 +5059,7 @@
         <v>T-28</v>
       </c>
       <c r="F68" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G68" t="s">
         <v>54</v>
@@ -5078,7 +5089,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5127,7 +5138,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5176,7 +5187,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5225,7 +5236,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5244,7 +5255,7 @@
         <v>T-58</v>
       </c>
       <c r="F72" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G72" t="s">
         <v>69</v>
@@ -5274,7 +5285,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5328,14 +5339,14 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>355</v>
+        <v>385</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D74" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="3"/>
@@ -5354,7 +5365,7 @@
         <v>46201</v>
       </c>
       <c r="K74" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O74">
         <v>73</v>
@@ -5374,14 +5385,14 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D75" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="3"/>
@@ -5391,7 +5402,7 @@
         <v>34</v>
       </c>
       <c r="G75" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H75" t="s">
         <v>64</v>
@@ -5400,7 +5411,7 @@
         <v>46202</v>
       </c>
       <c r="K75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O75">
         <v>74</v>
@@ -5420,14 +5431,14 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D76" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="3"/>
@@ -5446,7 +5457,7 @@
         <v>46202</v>
       </c>
       <c r="K76" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O76">
         <v>75</v>
@@ -5466,14 +5477,14 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D77" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
@@ -5492,7 +5503,7 @@
         <v>46202</v>
       </c>
       <c r="K77" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O77">
         <v>76</v>
@@ -5512,21 +5523,21 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D78" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F78" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G78" t="s">
         <v>54</v>
@@ -5538,7 +5549,7 @@
         <v>46203</v>
       </c>
       <c r="K78" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O78">
         <v>77</v>
@@ -5558,14 +5569,14 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>371</v>
+        <v>386</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D79" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
@@ -5584,7 +5595,7 @@
         <v>46203</v>
       </c>
       <c r="K79" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O79">
         <v>78</v>
@@ -5604,14 +5615,14 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D80" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
@@ -5630,7 +5641,7 @@
         <v>46203</v>
       </c>
       <c r="K80" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O80">
         <v>79</v>
@@ -5650,14 +5661,14 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>375</v>
+        <v>394</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D81" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
@@ -5676,7 +5687,7 @@
         <v>46204</v>
       </c>
       <c r="K81" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O81">
         <v>80</v>
@@ -5696,24 +5707,24 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D82" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F82" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="G82" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="H82" t="s">
         <v>62</v>
@@ -5722,7 +5733,7 @@
         <v>46204</v>
       </c>
       <c r="K82" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O82">
         <v>81</v>
@@ -5742,14 +5753,14 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D83" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="3"/>
@@ -5768,7 +5779,7 @@
         <v>46204</v>
       </c>
       <c r="K83" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O83">
         <v>82</v>
@@ -5788,14 +5799,14 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D84" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
@@ -5814,7 +5825,7 @@
         <v>46205</v>
       </c>
       <c r="K84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O84">
         <v>83</v>
@@ -5834,14 +5845,14 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D85" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
@@ -5860,7 +5871,7 @@
         <v>46205</v>
       </c>
       <c r="K85" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O85">
         <v>84</v>
@@ -5880,14 +5891,14 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D86" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
@@ -5906,7 +5917,7 @@
         <v>46205</v>
       </c>
       <c r="K86" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O86">
         <v>85</v>
@@ -5926,21 +5937,21 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D87" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F87" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G87" t="s">
         <v>69</v>
@@ -5952,7 +5963,7 @@
         <v>46206</v>
       </c>
       <c r="K87" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O87">
         <v>86</v>
@@ -5972,14 +5983,14 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D88" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
@@ -5998,7 +6009,7 @@
         <v>46206</v>
       </c>
       <c r="K88" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O88">
         <v>87</v>
@@ -6018,14 +6029,14 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D89" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="3"/>
@@ -6044,7 +6055,7 @@
         <v>46206</v>
       </c>
       <c r="K89" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O89">
         <v>88</v>
@@ -6064,14 +6075,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D90" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="3"/>
@@ -6090,7 +6101,7 @@
         <v>46207</v>
       </c>
       <c r="K90" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O90">
         <v>89</v>
@@ -6110,14 +6121,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D91" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="3"/>
@@ -6136,7 +6147,7 @@
         <v>46207</v>
       </c>
       <c r="K91" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O91">
         <v>90</v>
@@ -6156,21 +6167,21 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D92" t="s">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F92" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G92" t="s">
         <v>54</v>
@@ -6182,7 +6193,7 @@
         <v>46208</v>
       </c>
       <c r="K92" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O92">
         <v>91</v>
@@ -6202,14 +6213,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D93" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="3"/>
@@ -6228,7 +6239,7 @@
         <v>46208</v>
       </c>
       <c r="K93" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O93">
         <v>92</v>
@@ -6248,14 +6259,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D94" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="3"/>
@@ -6274,7 +6285,7 @@
         <v>46209</v>
       </c>
       <c r="K94" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O94">
         <v>93</v>
@@ -6283,7 +6294,7 @@
         <v>82</v>
       </c>
       <c r="Q94" t="s">
-        <v>432</v>
+        <v>376</v>
       </c>
       <c r="R94" t="s">
         <v>82</v>
@@ -6294,14 +6305,14 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D95" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="3"/>
@@ -6320,7 +6331,7 @@
         <v>46209</v>
       </c>
       <c r="K95" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
@@ -6328,14 +6339,14 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D96" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="3"/>
@@ -6354,7 +6365,7 @@
         <v>46210</v>
       </c>
       <c r="K96" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -6362,14 +6373,14 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D97" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="3"/>
@@ -6388,7 +6399,7 @@
         <v>46210</v>
       </c>
       <c r="K97" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -6396,14 +6407,14 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D98" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="3"/>
@@ -6413,7 +6424,7 @@
         <v>34</v>
       </c>
       <c r="G98" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H98" t="s">
         <v>64</v>
@@ -6422,7 +6433,7 @@
         <v>46212</v>
       </c>
       <c r="K98" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6430,14 +6441,14 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D99" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="3"/>
@@ -6456,7 +6467,7 @@
         <v>46212</v>
       </c>
       <c r="K99" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -6464,21 +6475,21 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D100" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F100" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G100" t="s">
         <v>69</v>
@@ -6490,7 +6501,7 @@
         <v>46212</v>
       </c>
       <c r="K100" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -6498,14 +6509,14 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D101" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="3"/>
@@ -6524,7 +6535,7 @@
         <v>46212</v>
       </c>
       <c r="K101" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -6532,14 +6543,14 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D102" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="3"/>
@@ -6558,7 +6569,7 @@
         <v>46217</v>
       </c>
       <c r="K102" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -6566,14 +6577,14 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D103" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="3"/>
@@ -6592,7 +6603,7 @@
         <v>46218</v>
       </c>
       <c r="K103" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -6600,21 +6611,21 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D104" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F104" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
       <c r="G104" t="s">
         <v>69</v>
@@ -6626,7 +6637,7 @@
         <v>46221</v>
       </c>
       <c r="K104" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -6634,21 +6645,21 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="2"/>
         <v>T-99</v>
       </c>
       <c r="D105" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="3"/>
         <v>T-99</v>
       </c>
       <c r="F105" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="G105" t="s">
         <v>54</v>
@@ -6660,18 +6671,13 @@
         <v>46222</v>
       </c>
       <c r="K105" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B76 B78:B105">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBC"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D78 D80:D105">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"tbc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
@@ -6679,8 +6685,13 @@
       <formula>"tbc"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D78 D80:D105">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"tbc"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBC"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6848,7 +6859,7 @@
         <v>248</v>
       </c>
       <c r="B9" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>

</xml_diff>